<commit_message>
comprobado el error gordo, obviamente es el piso que quedo filtrado por estar super lejos de la ciudad, y al añadirlo manualmente, pues en este comete mucho error. Vamos, que cuadno le pones algo fuera de contexto lo hace bastante mal. Aunque sí que está dentro de la cuadrícula
</commit_message>
<xml_diff>
--- a/9.0 XGBoost 5 pisos reales/Pisos_con_información.xlsx
+++ b/9.0 XGBoost 5 pisos reales/Pisos_con_información.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\TFG\9.0 XGBoost 5 pisos reales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA21BE69-08BA-40DA-BDFF-2E85EFB88414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C21D907-BDBB-40A5-BECE-1483CB75296A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2790" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t xml:space="preserve">Se vendió en el </t>
   </si>
@@ -187,6 +198,21 @@
   </si>
   <si>
     <t>ASSETID</t>
+  </si>
+  <si>
+    <t>PRED</t>
+  </si>
+  <si>
+    <t>REAL</t>
+  </si>
+  <si>
+    <t>IDEALISTA</t>
+  </si>
+  <si>
+    <t>Diff_Real</t>
+  </si>
+  <si>
+    <t>Diff_IDE</t>
   </si>
 </sst>
 </file>
@@ -513,15 +539,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP33"/>
+  <dimension ref="A1:AP45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AO30" sqref="AO30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="6" max="6" width="10.90625" customWidth="1"/>
+    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.35">
@@ -814,9 +842,6 @@
       <c r="B10">
         <v>201812</v>
       </c>
-      <c r="C10">
-        <v>268000</v>
-      </c>
       <c r="D10">
         <v>2791.666667</v>
       </c>
@@ -1233,9 +1258,6 @@
       <c r="B30">
         <v>201812</v>
       </c>
-      <c r="C30">
-        <v>493000</v>
-      </c>
       <c r="D30">
         <v>3763.3587790000001</v>
       </c>
@@ -1348,7 +1370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1357,6 +1379,118 @@
       </c>
       <c r="E33">
         <v>485000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F40" t="s">
+        <v>56</v>
+      </c>
+      <c r="G40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H40" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" t="s">
+        <v>57</v>
+      </c>
+      <c r="J40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F41">
+        <v>493000</v>
+      </c>
+      <c r="G41">
+        <v>485000</v>
+      </c>
+      <c r="H41">
+        <v>641511.9</v>
+      </c>
+      <c r="I41">
+        <f>(100*(G41/H41))</f>
+        <v>75.602650550987434</v>
+      </c>
+      <c r="J41">
+        <f>(100*(F41/H41))</f>
+        <v>76.84970458069445</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F42">
+        <v>1665000</v>
+      </c>
+      <c r="G42">
+        <v>1500000</v>
+      </c>
+      <c r="H42">
+        <v>1750086.6</v>
+      </c>
+      <c r="I42">
+        <f t="shared" ref="I42:I45" si="0">(100*(G42/H42))</f>
+        <v>85.710044291522479</v>
+      </c>
+      <c r="J42">
+        <f t="shared" ref="J42:J45" si="1">(100*(F42/H42))</f>
+        <v>95.138149163589958</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F43">
+        <v>153000</v>
+      </c>
+      <c r="G43">
+        <v>149900</v>
+      </c>
+      <c r="H43">
+        <v>186867.78</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="0"/>
+        <v>80.217146048398504</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="1"/>
+        <v>81.876073018045176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F44">
+        <v>738000</v>
+      </c>
+      <c r="G44">
+        <v>600000</v>
+      </c>
+      <c r="H44">
+        <v>743707.94</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="0"/>
+        <v>80.676831284065628</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="1"/>
+        <v>99.232502479400736</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F45">
+        <v>268000</v>
+      </c>
+      <c r="G45">
+        <v>250000</v>
+      </c>
+      <c r="H45">
+        <v>325048.15999999997</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="0"/>
+        <v>76.911679795387869</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="1"/>
+        <v>82.449320740655793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
para que se quede todo guardado
</commit_message>
<xml_diff>
--- a/9.0 XGBoost 5 pisos reales/Pisos_con_información.xlsx
+++ b/9.0 XGBoost 5 pisos reales/Pisos_con_información.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costa\Desktop\TFG\9.0 XGBoost 5 pisos reales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C21D907-BDBB-40A5-BECE-1483CB75296A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1899E6-8776-4A7E-B912-056074041972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2790" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t xml:space="preserve">Se vendió en el </t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Diff_IDE</t>
+  </si>
+  <si>
+    <t>PRED VERD</t>
   </si>
 </sst>
 </file>
@@ -539,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AP45"/>
+  <dimension ref="A1:AP48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H45" sqref="H40:H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,6 +553,7 @@
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="6" max="6" width="10.90625" customWidth="1"/>
     <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.35">
@@ -1370,7 +1374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1381,7 +1385,7 @@
         <v>485000</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F40" t="s">
         <v>56</v>
       </c>
@@ -1392,13 +1396,16 @@
         <v>54</v>
       </c>
       <c r="I40" t="s">
+        <v>59</v>
+      </c>
+      <c r="J40" t="s">
         <v>57</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F41">
         <v>493000</v>
       </c>
@@ -1409,15 +1416,28 @@
         <v>641511.9</v>
       </c>
       <c r="I41">
+        <v>691651.5</v>
+      </c>
+      <c r="J41">
         <f>(100*(G41/H41))</f>
         <v>75.602650550987434</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <f>(100*(F41/H41))</f>
         <v>76.84970458069445</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L41">
+        <f>(100*(F41/I41))</f>
+        <v>71.278671411830956</v>
+      </c>
+      <c r="M41">
+        <v>13</v>
+      </c>
+      <c r="N41">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F42">
         <v>1665000</v>
       </c>
@@ -1428,15 +1448,28 @@
         <v>1750086.6</v>
       </c>
       <c r="I42">
-        <f t="shared" ref="I42:I45" si="0">(100*(G42/H42))</f>
+        <v>1628478.6</v>
+      </c>
+      <c r="J42">
+        <f>(100*(G42/H42))</f>
         <v>85.710044291522479</v>
       </c>
-      <c r="J42">
-        <f t="shared" ref="J42:J45" si="1">(100*(F42/H42))</f>
+      <c r="K42">
+        <f>(100*(F42/H42))</f>
         <v>95.138149163589958</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L42">
+        <f>(100*(F42/I42))</f>
+        <v>102.24266993744959</v>
+      </c>
+      <c r="M42">
+        <v>5</v>
+      </c>
+      <c r="N42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F43">
         <v>153000</v>
       </c>
@@ -1447,15 +1480,28 @@
         <v>186867.78</v>
       </c>
       <c r="I43">
-        <f t="shared" si="0"/>
+        <v>217975.98</v>
+      </c>
+      <c r="J43">
+        <f>(100*(G43/H43))</f>
         <v>80.217146048398504</v>
       </c>
-      <c r="J43">
-        <f t="shared" si="1"/>
+      <c r="K43">
+        <f>(100*(F43/H43))</f>
         <v>81.876073018045176</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L43">
+        <f>(100*(F43/I43))</f>
+        <v>70.191220151871775</v>
+      </c>
+      <c r="M43">
+        <v>18</v>
+      </c>
+      <c r="N43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F44">
         <v>738000</v>
       </c>
@@ -1466,15 +1512,28 @@
         <v>743707.94</v>
       </c>
       <c r="I44">
-        <f t="shared" si="0"/>
+        <v>713190.40000000002</v>
+      </c>
+      <c r="J44">
+        <f>(100*(G44/H44))</f>
         <v>80.676831284065628</v>
       </c>
-      <c r="J44">
-        <f t="shared" si="1"/>
+      <c r="K44">
+        <f>(100*(F44/H44))</f>
         <v>99.232502479400736</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L44">
+        <f>(100*(F44/I44))</f>
+        <v>103.47867834452063</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F45">
         <v>268000</v>
       </c>
@@ -1485,12 +1544,45 @@
         <v>325048.15999999997</v>
       </c>
       <c r="I45">
-        <f t="shared" si="0"/>
+        <v>320622</v>
+      </c>
+      <c r="J45">
+        <f>(100*(G45/H45))</f>
         <v>76.911679795387869</v>
       </c>
-      <c r="J45">
-        <f t="shared" si="1"/>
+      <c r="K45">
+        <f>(100*(F45/H45))</f>
         <v>82.449320740655793</v>
+      </c>
+      <c r="L45">
+        <f>(100*(F45/I45))</f>
+        <v>83.587526744889615</v>
+      </c>
+      <c r="M45">
+        <v>17</v>
+      </c>
+      <c r="N45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M46">
+        <f>(0.2*(M41+M42+M43+M44+M45))</f>
+        <v>10.8</v>
+      </c>
+      <c r="N46">
+        <f>(0.2*(N41+N42+N43+N44+N45))</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="M48">
+        <f>(0.2*(M43+M44+M45+M46))</f>
+        <v>9.36</v>
+      </c>
+      <c r="N48">
+        <f>(0.2*(N43+N44+N45+N46))</f>
+        <v>12.600000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>